<commit_message>
Recursion technique Implemented for Traveling Salesman Problem.
</commit_message>
<xml_diff>
--- a/V101/Accountability Sheet.xlsx
+++ b/V101/Accountability Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saitejsunkara/Desktop/Final-Projects/PSA-Final-Project/V101/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F0660A-9C23-064F-84B4-B8757DE7556F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383A7EB7-BA19-BD4C-94C9-61B5B7F9E84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D57C6A6E-9C01-114D-A0CB-9523281CCD6A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
   <si>
     <t>Progress</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>Performance Analysis</t>
+  </si>
+  <si>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cY4HiiFHO1o</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=bSaBmXFym30</t>
   </si>
 </sst>
 </file>
@@ -500,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4C35A5-7693-F241-9BE6-3AA69C33C803}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,10 +522,11 @@
     <col min="3" max="4" width="24.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.1640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="32.83203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -535,8 +545,11 @@
       <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -555,28 +568,34 @@
       <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="G3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5">
         <v>45029</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -596,7 +615,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -616,7 +635,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -636,7 +655,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -656,7 +675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -676,7 +695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -696,7 +715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -716,7 +735,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -736,7 +755,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -756,7 +775,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -776,7 +795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -796,7 +815,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Added Accountability tasks and Workspaces
</commit_message>
<xml_diff>
--- a/V101/Accountability Sheet.xlsx
+++ b/V101/Accountability Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saitejsunkara/Desktop/Final-Projects/PSA-Final-Project/V101/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EA917D-2A18-7444-A22F-FE4A7342F774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC87EDF1-7529-6142-9C11-E75B8A12252B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D57C6A6E-9C01-114D-A0CB-9523281CCD6A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{D57C6A6E-9C01-114D-A0CB-9523281CCD6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
   <si>
     <t>Progress</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Performance Analysis</t>
   </si>
   <si>
-    <t>Sources</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=cY4HiiFHO1o</t>
   </si>
   <si>
@@ -132,6 +129,12 @@
   </si>
   <si>
     <t xml:space="preserve">Dynamic Programming Implementation (O(n^2*2^n) time complexity) </t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=JE0JE8ce1V0</t>
   </si>
 </sst>
 </file>
@@ -181,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,12 +199,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -521,7 +518,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,7 +528,7 @@
     <col min="3" max="4" width="24.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="47" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -555,7 +552,7 @@
         <v>12</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -578,7 +575,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -601,7 +598,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -629,7 +626,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
@@ -645,23 +642,26 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="7">
+      <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5">
         <v>45029</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>